<commit_message>
set up full and mem for ccanada
</commit_message>
<xml_diff>
--- a/pendulum/neg_full_pendulum/neg_full_raw_data.xlsx
+++ b/pendulum/neg_full_pendulum/neg_full_raw_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/neg_full_pendulum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2CA6B8-8040-1A4F-840F-0471C3C364FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACDC061-909C-BB4A-B8D2-7AF0247D1C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -376,9 +376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>